<commit_message>
add egypt terms top
</commit_message>
<xml_diff>
--- a/gnip/rules/Pull specs for GNIP (with operators).xlsx
+++ b/gnip/rules/Pull specs for GNIP (with operators).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="0" windowWidth="25600" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pull specs for GNIP (with opera" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -781,37 +781,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" s="3" customFormat="1">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>39736</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>39737</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>39742</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>39743</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>